<commit_message>
Added ISO codes for subregions.
</commit_message>
<xml_diff>
--- a/data/Combined Country Subdivision Table.xlsx
+++ b/data/Combined Country Subdivision Table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proginoskes\Cloud Storage\Google Drive\Data\World\Country Subdivisions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proginoskes\Documents\GitHub\Country-Subdivisions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5285" uniqueCount="1347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5579" uniqueCount="1437">
   <si>
     <t>Russia</t>
   </si>
@@ -4065,6 +4065,276 @@
   </si>
   <si>
     <t>Statistics Bureau of Japan|Geographical Survey Institute of Japan</t>
+  </si>
+  <si>
+    <t>Abu Dhabi</t>
+  </si>
+  <si>
+    <t>Ajman</t>
+  </si>
+  <si>
+    <t>Dubai</t>
+  </si>
+  <si>
+    <t>Fujairah</t>
+  </si>
+  <si>
+    <t>Ras al-Khaimah</t>
+  </si>
+  <si>
+    <t>Sharjah</t>
+  </si>
+  <si>
+    <t>Umm al-Quwain</t>
+  </si>
+  <si>
+    <t>Emirate</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>UAE</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/United_Arab_Emirates#Political_divisions</t>
+  </si>
+  <si>
+    <t>AE-AZ</t>
+  </si>
+  <si>
+    <t>AE-AJ</t>
+  </si>
+  <si>
+    <t>AE-FU</t>
+  </si>
+  <si>
+    <t>AE-SH</t>
+  </si>
+  <si>
+    <t>AE-DU</t>
+  </si>
+  <si>
+    <t>AE-RK</t>
+  </si>
+  <si>
+    <t>AE-UQ</t>
+  </si>
+  <si>
+    <t>Badakhshan</t>
+  </si>
+  <si>
+    <t>AF-BDS</t>
+  </si>
+  <si>
+    <t>Badghis</t>
+  </si>
+  <si>
+    <t>AF-BDG</t>
+  </si>
+  <si>
+    <t>Baghlan</t>
+  </si>
+  <si>
+    <t>AF-BGL</t>
+  </si>
+  <si>
+    <t>Balkh</t>
+  </si>
+  <si>
+    <t>AF-BAL</t>
+  </si>
+  <si>
+    <t>Bamyan</t>
+  </si>
+  <si>
+    <t>AF-BAM</t>
+  </si>
+  <si>
+    <t>Daykundi</t>
+  </si>
+  <si>
+    <t>AF-DAY</t>
+  </si>
+  <si>
+    <t>Farah</t>
+  </si>
+  <si>
+    <t>AF-FRA</t>
+  </si>
+  <si>
+    <t>Faryab</t>
+  </si>
+  <si>
+    <t>AF-FYB</t>
+  </si>
+  <si>
+    <t>Ghazni</t>
+  </si>
+  <si>
+    <t>AF-GHA</t>
+  </si>
+  <si>
+    <t>Ghor</t>
+  </si>
+  <si>
+    <t>AF-GHO</t>
+  </si>
+  <si>
+    <t>Helmand</t>
+  </si>
+  <si>
+    <t>AF-HEL</t>
+  </si>
+  <si>
+    <t>Herat</t>
+  </si>
+  <si>
+    <t>AF-HER</t>
+  </si>
+  <si>
+    <t>Jowzjan</t>
+  </si>
+  <si>
+    <t>AF-JOW</t>
+  </si>
+  <si>
+    <t>Kabul</t>
+  </si>
+  <si>
+    <t>AF-KAB</t>
+  </si>
+  <si>
+    <t>Kandahar</t>
+  </si>
+  <si>
+    <t>AF-KAN</t>
+  </si>
+  <si>
+    <t>Kapisa</t>
+  </si>
+  <si>
+    <t>AF-KAP</t>
+  </si>
+  <si>
+    <t>Khost</t>
+  </si>
+  <si>
+    <t>AF-KHO</t>
+  </si>
+  <si>
+    <t>Kunar</t>
+  </si>
+  <si>
+    <t>AF-KNR</t>
+  </si>
+  <si>
+    <t>Kunduz</t>
+  </si>
+  <si>
+    <t>AF-KDZ</t>
+  </si>
+  <si>
+    <t>Laghman</t>
+  </si>
+  <si>
+    <t>AF-LAG</t>
+  </si>
+  <si>
+    <t>Logar</t>
+  </si>
+  <si>
+    <t>AF-LOG</t>
+  </si>
+  <si>
+    <t>Maidan Wardak</t>
+  </si>
+  <si>
+    <t>AF-WAR</t>
+  </si>
+  <si>
+    <t>Nangarhar</t>
+  </si>
+  <si>
+    <t>AF-NAN</t>
+  </si>
+  <si>
+    <t>Nimruz</t>
+  </si>
+  <si>
+    <t>AF-NIM</t>
+  </si>
+  <si>
+    <t>Nuristan</t>
+  </si>
+  <si>
+    <t>AF-NUR</t>
+  </si>
+  <si>
+    <t>Paktia</t>
+  </si>
+  <si>
+    <t>AF-PIA</t>
+  </si>
+  <si>
+    <t>Paktika</t>
+  </si>
+  <si>
+    <t>AF-PKA</t>
+  </si>
+  <si>
+    <t>Panjshir</t>
+  </si>
+  <si>
+    <t>AF-PAN</t>
+  </si>
+  <si>
+    <t>Parwan</t>
+  </si>
+  <si>
+    <t>AF-PAR</t>
+  </si>
+  <si>
+    <t>Samangan</t>
+  </si>
+  <si>
+    <t>AF-SAM</t>
+  </si>
+  <si>
+    <t>Sar-e Pol</t>
+  </si>
+  <si>
+    <t>AF-SAR</t>
+  </si>
+  <si>
+    <t>Takhar</t>
+  </si>
+  <si>
+    <t>AF-TAK</t>
+  </si>
+  <si>
+    <t>Urozgan</t>
+  </si>
+  <si>
+    <t>AF-URU</t>
+  </si>
+  <si>
+    <t>Zabul</t>
+  </si>
+  <si>
+    <t>AF-ZAB</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>AFG</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Provinces_of_Afghanistan</t>
   </si>
 </sst>
 </file>
@@ -4113,7 +4383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4133,6 +4403,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4447,11 +4720,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q666"/>
+  <dimension ref="A1:Q707"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J77" sqref="J77"/>
+      <pane ySplit="1" topLeftCell="A673" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K695" sqref="K695"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30365,6 +30638,1503 @@
         <v>1346</v>
       </c>
     </row>
+    <row r="667" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A667">
+        <v>2008</v>
+      </c>
+      <c r="B667" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C667" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D667" t="s">
+        <v>1358</v>
+      </c>
+      <c r="E667" t="s">
+        <v>99</v>
+      </c>
+      <c r="F667" t="s">
+        <v>1347</v>
+      </c>
+      <c r="G667" t="s">
+        <v>1354</v>
+      </c>
+      <c r="H667" s="1">
+        <v>67340</v>
+      </c>
+      <c r="I667" s="11">
+        <v>1548655</v>
+      </c>
+      <c r="J667" s="2">
+        <f>I667/H667</f>
+        <v>22.997549747549748</v>
+      </c>
+      <c r="K667" t="s">
+        <v>1357</v>
+      </c>
+      <c r="L667" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="668" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A668">
+        <v>2008</v>
+      </c>
+      <c r="B668" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C668" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D668" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E668" t="s">
+        <v>99</v>
+      </c>
+      <c r="F668" t="s">
+        <v>1348</v>
+      </c>
+      <c r="G668" t="s">
+        <v>1354</v>
+      </c>
+      <c r="H668">
+        <v>259</v>
+      </c>
+      <c r="I668" s="1">
+        <v>372923</v>
+      </c>
+      <c r="J668" s="2">
+        <f t="shared" ref="J668:J673" si="10">I668/H668</f>
+        <v>1439.8571428571429</v>
+      </c>
+      <c r="K668" t="s">
+        <v>1357</v>
+      </c>
+      <c r="L668" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="669" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A669">
+        <v>2008</v>
+      </c>
+      <c r="B669" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C669" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D669" t="s">
+        <v>1362</v>
+      </c>
+      <c r="E669" t="s">
+        <v>99</v>
+      </c>
+      <c r="F669" t="s">
+        <v>1349</v>
+      </c>
+      <c r="G669" t="s">
+        <v>1354</v>
+      </c>
+      <c r="H669" s="1">
+        <v>3885</v>
+      </c>
+      <c r="I669" s="1">
+        <v>1770533</v>
+      </c>
+      <c r="J669" s="2">
+        <f t="shared" si="10"/>
+        <v>455.73564993564992</v>
+      </c>
+      <c r="K669" t="s">
+        <v>1357</v>
+      </c>
+      <c r="L669" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="670" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A670">
+        <v>2008</v>
+      </c>
+      <c r="B670" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C670" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D670" t="s">
+        <v>1360</v>
+      </c>
+      <c r="E670" t="s">
+        <v>99</v>
+      </c>
+      <c r="F670" t="s">
+        <v>1350</v>
+      </c>
+      <c r="G670" t="s">
+        <v>1354</v>
+      </c>
+      <c r="H670" s="1">
+        <v>1165</v>
+      </c>
+      <c r="I670" s="1">
+        <v>137940</v>
+      </c>
+      <c r="J670" s="2">
+        <f t="shared" si="10"/>
+        <v>118.40343347639485</v>
+      </c>
+      <c r="K670" t="s">
+        <v>1357</v>
+      </c>
+      <c r="L670" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="671" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A671">
+        <v>2008</v>
+      </c>
+      <c r="B671" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C671" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D671" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E671" t="s">
+        <v>99</v>
+      </c>
+      <c r="F671" t="s">
+        <v>1351</v>
+      </c>
+      <c r="G671" t="s">
+        <v>1354</v>
+      </c>
+      <c r="H671" s="1">
+        <v>1684</v>
+      </c>
+      <c r="I671" s="1">
+        <v>171903</v>
+      </c>
+      <c r="J671" s="2">
+        <f t="shared" si="10"/>
+        <v>102.08016627078385</v>
+      </c>
+      <c r="K671" t="s">
+        <v>1357</v>
+      </c>
+      <c r="L671" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="672" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A672">
+        <v>2008</v>
+      </c>
+      <c r="B672" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C672" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D672" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E672" t="s">
+        <v>99</v>
+      </c>
+      <c r="F672" t="s">
+        <v>1352</v>
+      </c>
+      <c r="G672" t="s">
+        <v>1354</v>
+      </c>
+      <c r="H672" s="1">
+        <v>2590</v>
+      </c>
+      <c r="I672" s="1">
+        <v>895252</v>
+      </c>
+      <c r="J672" s="2">
+        <f t="shared" si="10"/>
+        <v>345.65714285714284</v>
+      </c>
+      <c r="K672" t="s">
+        <v>1357</v>
+      </c>
+      <c r="L672" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="673" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A673">
+        <v>2008</v>
+      </c>
+      <c r="B673" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C673" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D673" t="s">
+        <v>1364</v>
+      </c>
+      <c r="E673" t="s">
+        <v>99</v>
+      </c>
+      <c r="F673" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G673" t="s">
+        <v>1354</v>
+      </c>
+      <c r="H673">
+        <v>777</v>
+      </c>
+      <c r="I673" s="1">
+        <v>69936</v>
+      </c>
+      <c r="J673" s="2">
+        <f t="shared" si="10"/>
+        <v>90.007722007722009</v>
+      </c>
+      <c r="K673" t="s">
+        <v>1357</v>
+      </c>
+      <c r="L673" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="674" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A674">
+        <v>2015</v>
+      </c>
+      <c r="B674" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C674" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D674" s="3" t="s">
+        <v>1366</v>
+      </c>
+      <c r="F674" t="s">
+        <v>1365</v>
+      </c>
+      <c r="G674" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H674" s="1">
+        <v>44059</v>
+      </c>
+      <c r="I674" s="2">
+        <v>950953</v>
+      </c>
+      <c r="J674" s="2">
+        <f>I674/H674</f>
+        <v>21.583626500828434</v>
+      </c>
+      <c r="K674" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L674" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="675" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A675">
+        <v>2015</v>
+      </c>
+      <c r="B675" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C675" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D675" s="3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="F675" t="s">
+        <v>1367</v>
+      </c>
+      <c r="G675" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H675" s="1">
+        <v>20591</v>
+      </c>
+      <c r="I675" s="2">
+        <v>495958</v>
+      </c>
+      <c r="J675" s="2">
+        <f t="shared" ref="J675:J707" si="11">I675/H675</f>
+        <v>24.086154145014813</v>
+      </c>
+      <c r="K675" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L675" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="676" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A676">
+        <v>2015</v>
+      </c>
+      <c r="B676" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C676" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D676" s="3" t="s">
+        <v>1370</v>
+      </c>
+      <c r="F676" t="s">
+        <v>1369</v>
+      </c>
+      <c r="G676" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H676" s="1">
+        <v>21118</v>
+      </c>
+      <c r="I676" s="2">
+        <v>910784</v>
+      </c>
+      <c r="J676" s="2">
+        <f t="shared" si="11"/>
+        <v>43.12832654607444</v>
+      </c>
+      <c r="K676" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L676" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="677" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A677">
+        <v>2015</v>
+      </c>
+      <c r="B677" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C677" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D677" s="3" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F677" t="s">
+        <v>1371</v>
+      </c>
+      <c r="G677" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H677" s="1">
+        <v>17249</v>
+      </c>
+      <c r="I677" s="2">
+        <v>1325659</v>
+      </c>
+      <c r="J677" s="2">
+        <f t="shared" si="11"/>
+        <v>76.854252420430171</v>
+      </c>
+      <c r="K677" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L677" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="678" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A678">
+        <v>2015</v>
+      </c>
+      <c r="B678" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C678" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D678" s="3" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F678" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G678" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H678" s="1">
+        <v>14175</v>
+      </c>
+      <c r="I678" s="2">
+        <v>747218</v>
+      </c>
+      <c r="J678" s="2">
+        <f t="shared" si="11"/>
+        <v>52.713791887125218</v>
+      </c>
+      <c r="K678" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L678" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="679" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A679">
+        <v>2015</v>
+      </c>
+      <c r="B679" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C679" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D679" s="3" t="s">
+        <v>1376</v>
+      </c>
+      <c r="F679" t="s">
+        <v>1375</v>
+      </c>
+      <c r="G679" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H679" s="1">
+        <v>18088</v>
+      </c>
+      <c r="I679" s="2">
+        <v>924339</v>
+      </c>
+      <c r="J679" s="2">
+        <f t="shared" si="11"/>
+        <v>51.102333038478548</v>
+      </c>
+      <c r="K679" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L679" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="680" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A680">
+        <v>2015</v>
+      </c>
+      <c r="B680" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C680" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D680" s="3" t="s">
+        <v>1378</v>
+      </c>
+      <c r="F680" t="s">
+        <v>1377</v>
+      </c>
+      <c r="G680" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H680" s="1">
+        <v>48471</v>
+      </c>
+      <c r="I680" s="2">
+        <v>507405</v>
+      </c>
+      <c r="J680" s="2">
+        <f t="shared" si="11"/>
+        <v>10.468218109797611</v>
+      </c>
+      <c r="K680" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L680" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="681" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A681">
+        <v>2015</v>
+      </c>
+      <c r="B681" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C681" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D681" s="3" t="s">
+        <v>1380</v>
+      </c>
+      <c r="F681" t="s">
+        <v>1379</v>
+      </c>
+      <c r="G681" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H681" s="1">
+        <v>20293</v>
+      </c>
+      <c r="I681" s="2">
+        <v>998147</v>
+      </c>
+      <c r="J681" s="2">
+        <f t="shared" si="11"/>
+        <v>49.186763908736999</v>
+      </c>
+      <c r="K681" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L681" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="682" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A682">
+        <v>2015</v>
+      </c>
+      <c r="B682" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C682" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D682" s="3" t="s">
+        <v>1382</v>
+      </c>
+      <c r="F682" t="s">
+        <v>1381</v>
+      </c>
+      <c r="G682" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H682" s="1">
+        <v>22915</v>
+      </c>
+      <c r="I682" s="2">
+        <v>1228831</v>
+      </c>
+      <c r="J682" s="2">
+        <f t="shared" si="11"/>
+        <v>53.625616408466072</v>
+      </c>
+      <c r="K682" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L682" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="683" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A683">
+        <v>2015</v>
+      </c>
+      <c r="B683" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C683" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D683" s="3" t="s">
+        <v>1384</v>
+      </c>
+      <c r="F683" t="s">
+        <v>1383</v>
+      </c>
+      <c r="G683" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H683" s="1">
+        <v>36479</v>
+      </c>
+      <c r="I683" s="2">
+        <v>790296</v>
+      </c>
+      <c r="J683" s="2">
+        <f t="shared" si="11"/>
+        <v>21.664409660352533</v>
+      </c>
+      <c r="K683" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L683" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="684" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A684">
+        <v>2015</v>
+      </c>
+      <c r="B684" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C684" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D684" s="3" t="s">
+        <v>1386</v>
+      </c>
+      <c r="F684" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G684" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H684" s="1">
+        <v>58584</v>
+      </c>
+      <c r="I684" s="2">
+        <v>924711</v>
+      </c>
+      <c r="J684" s="2">
+        <f t="shared" si="11"/>
+        <v>15.784360917656699</v>
+      </c>
+      <c r="K684" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L684" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="685" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A685">
+        <v>2015</v>
+      </c>
+      <c r="B685" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C685" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D685" s="3" t="s">
+        <v>1388</v>
+      </c>
+      <c r="F685" t="s">
+        <v>1387</v>
+      </c>
+      <c r="G685" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H685" s="1">
+        <v>54778</v>
+      </c>
+      <c r="I685" s="2">
+        <v>1890202</v>
+      </c>
+      <c r="J685" s="2">
+        <f t="shared" si="11"/>
+        <v>34.506590236956441</v>
+      </c>
+      <c r="K685" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L685" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="686" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A686">
+        <v>2015</v>
+      </c>
+      <c r="B686" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C686" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D686" s="3" t="s">
+        <v>1390</v>
+      </c>
+      <c r="F686" t="s">
+        <v>1389</v>
+      </c>
+      <c r="G686" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H686" s="1">
+        <v>11798</v>
+      </c>
+      <c r="I686" s="2">
+        <v>540255</v>
+      </c>
+      <c r="J686" s="2">
+        <f t="shared" si="11"/>
+        <v>45.792083403966771</v>
+      </c>
+      <c r="K686" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L686" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="687" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A687">
+        <v>2015</v>
+      </c>
+      <c r="B687" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C687" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D687" s="3" t="s">
+        <v>1392</v>
+      </c>
+      <c r="F687" t="s">
+        <v>1391</v>
+      </c>
+      <c r="G687" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H687" s="1">
+        <v>4462</v>
+      </c>
+      <c r="I687" s="2">
+        <v>4372977</v>
+      </c>
+      <c r="J687" s="2">
+        <f t="shared" si="11"/>
+        <v>980.04863290004482</v>
+      </c>
+      <c r="K687" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L687" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="688" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A688">
+        <v>2015</v>
+      </c>
+      <c r="B688" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C688" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D688" s="3" t="s">
+        <v>1394</v>
+      </c>
+      <c r="F688" t="s">
+        <v>1393</v>
+      </c>
+      <c r="G688" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H688" s="1">
+        <v>54022</v>
+      </c>
+      <c r="I688" s="2">
+        <v>1226593</v>
+      </c>
+      <c r="J688" s="2">
+        <f t="shared" si="11"/>
+        <v>22.705434822849949</v>
+      </c>
+      <c r="K688" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L688" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="689" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A689">
+        <v>2015</v>
+      </c>
+      <c r="B689" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C689" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D689" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="F689" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G689" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H689" s="1">
+        <v>1842</v>
+      </c>
+      <c r="I689" s="2">
+        <v>441010</v>
+      </c>
+      <c r="J689" s="2">
+        <f t="shared" si="11"/>
+        <v>239.41910966340933</v>
+      </c>
+      <c r="K689" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L689" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="690" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A690">
+        <v>2015</v>
+      </c>
+      <c r="B690" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C690" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D690" s="3" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F690" t="s">
+        <v>1397</v>
+      </c>
+      <c r="G690" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H690" s="1">
+        <v>4152</v>
+      </c>
+      <c r="I690" s="2">
+        <v>574582</v>
+      </c>
+      <c r="J690" s="2">
+        <f t="shared" si="11"/>
+        <v>138.38680154142583</v>
+      </c>
+      <c r="K690" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L690" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="691" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A691">
+        <v>2015</v>
+      </c>
+      <c r="B691" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C691" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D691" s="3" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F691" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G691" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H691" s="1">
+        <v>4942</v>
+      </c>
+      <c r="I691" s="2">
+        <v>450652</v>
+      </c>
+      <c r="J691" s="2">
+        <f t="shared" si="11"/>
+        <v>91.188182921893969</v>
+      </c>
+      <c r="K691" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L691" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="692" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A692">
+        <v>2015</v>
+      </c>
+      <c r="B692" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C692" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D692" s="3" t="s">
+        <v>1402</v>
+      </c>
+      <c r="F692" t="s">
+        <v>1401</v>
+      </c>
+      <c r="G692" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H692" s="1">
+        <v>8040</v>
+      </c>
+      <c r="I692" s="2">
+        <v>1010037</v>
+      </c>
+      <c r="J692" s="2">
+        <f t="shared" si="11"/>
+        <v>125.62649253731344</v>
+      </c>
+      <c r="K692" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L692" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="693" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A693">
+        <v>2015</v>
+      </c>
+      <c r="B693" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C693" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D693" s="3" t="s">
+        <v>1404</v>
+      </c>
+      <c r="F693" t="s">
+        <v>1403</v>
+      </c>
+      <c r="G693" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H693" s="1">
+        <v>3843</v>
+      </c>
+      <c r="I693" s="2">
+        <v>445588</v>
+      </c>
+      <c r="J693" s="2">
+        <f t="shared" si="11"/>
+        <v>115.9479573250065</v>
+      </c>
+      <c r="K693" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L693" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="694" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A694">
+        <v>2015</v>
+      </c>
+      <c r="B694" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C694" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D694" s="3" t="s">
+        <v>1406</v>
+      </c>
+      <c r="F694" t="s">
+        <v>1405</v>
+      </c>
+      <c r="G694" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H694" s="1">
+        <v>3880</v>
+      </c>
+      <c r="I694" s="2">
+        <v>392045</v>
+      </c>
+      <c r="J694" s="2">
+        <f t="shared" si="11"/>
+        <v>101.04252577319588</v>
+      </c>
+      <c r="K694" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L694" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="695" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A695">
+        <v>2015</v>
+      </c>
+      <c r="B695" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C695" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D695" s="3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="F695" t="s">
+        <v>1407</v>
+      </c>
+      <c r="G695" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H695" s="1">
+        <v>9934</v>
+      </c>
+      <c r="I695" s="2">
+        <v>596287</v>
+      </c>
+      <c r="J695" s="2">
+        <f t="shared" si="11"/>
+        <v>60.024864103080333</v>
+      </c>
+      <c r="K695" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L695" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="696" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A696">
+        <v>2015</v>
+      </c>
+      <c r="B696" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C696" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D696" s="3" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F696" t="s">
+        <v>1409</v>
+      </c>
+      <c r="G696" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H696" s="1">
+        <v>7727</v>
+      </c>
+      <c r="I696" s="2">
+        <v>1517388</v>
+      </c>
+      <c r="J696" s="2">
+        <f t="shared" si="11"/>
+        <v>196.37478969845995</v>
+      </c>
+      <c r="K696" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L696" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="697" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A697">
+        <v>2015</v>
+      </c>
+      <c r="B697" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C697" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D697" s="3" t="s">
+        <v>1412</v>
+      </c>
+      <c r="F697" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G697" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H697" s="1">
+        <v>41005</v>
+      </c>
+      <c r="I697" s="2">
+        <v>164978</v>
+      </c>
+      <c r="J697" s="2">
+        <f t="shared" si="11"/>
+        <v>4.0233630045116451</v>
+      </c>
+      <c r="K697" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L697" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="698" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A698">
+        <v>2015</v>
+      </c>
+      <c r="B698" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C698" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D698" s="3" t="s">
+        <v>1414</v>
+      </c>
+      <c r="F698" t="s">
+        <v>1413</v>
+      </c>
+      <c r="G698" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H698" s="1">
+        <v>9225</v>
+      </c>
+      <c r="I698" s="2">
+        <v>147967</v>
+      </c>
+      <c r="J698" s="2">
+        <f t="shared" si="11"/>
+        <v>16.03978319783198</v>
+      </c>
+      <c r="K698" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L698" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="699" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A699">
+        <v>2015</v>
+      </c>
+      <c r="B699" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C699" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D699" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F699" t="s">
+        <v>1415</v>
+      </c>
+      <c r="G699" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H699" s="1">
+        <v>6432</v>
+      </c>
+      <c r="I699" s="2">
+        <v>551987</v>
+      </c>
+      <c r="J699" s="2">
+        <f t="shared" si="11"/>
+        <v>85.818874378109456</v>
+      </c>
+      <c r="K699" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L699" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="700" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A700">
+        <v>2015</v>
+      </c>
+      <c r="B700" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C700" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D700" s="3" t="s">
+        <v>1418</v>
+      </c>
+      <c r="F700" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G700" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H700" s="1">
+        <v>19482</v>
+      </c>
+      <c r="I700" s="2">
+        <v>434742</v>
+      </c>
+      <c r="J700" s="2">
+        <f t="shared" si="11"/>
+        <v>22.315060055435787</v>
+      </c>
+      <c r="K700" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L700" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="701" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A701">
+        <v>2015</v>
+      </c>
+      <c r="B701" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C701" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D701" s="3" t="s">
+        <v>1420</v>
+      </c>
+      <c r="F701" t="s">
+        <v>1419</v>
+      </c>
+      <c r="G701" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H701" s="1">
+        <v>3610</v>
+      </c>
+      <c r="I701" s="2">
+        <v>153487</v>
+      </c>
+      <c r="J701" s="2">
+        <f t="shared" si="11"/>
+        <v>42.51717451523546</v>
+      </c>
+      <c r="K701" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L701" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="702" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A702">
+        <v>2015</v>
+      </c>
+      <c r="B702" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C702" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D702" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="F702" t="s">
+        <v>1421</v>
+      </c>
+      <c r="G702" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H702" s="1">
+        <v>5974</v>
+      </c>
+      <c r="I702" s="2">
+        <v>664502</v>
+      </c>
+      <c r="J702" s="2">
+        <f t="shared" si="11"/>
+        <v>111.23234014060931</v>
+      </c>
+      <c r="K702" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L702" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="703" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A703">
+        <v>2015</v>
+      </c>
+      <c r="B703" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C703" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D703" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="F703" t="s">
+        <v>1423</v>
+      </c>
+      <c r="G703" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H703" s="1">
+        <v>11262</v>
+      </c>
+      <c r="I703" s="2">
+        <v>387928</v>
+      </c>
+      <c r="J703" s="2">
+        <f t="shared" si="11"/>
+        <v>34.445746759012607</v>
+      </c>
+      <c r="K703" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L703" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="704" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A704">
+        <v>2015</v>
+      </c>
+      <c r="B704" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C704" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D704" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="F704" t="s">
+        <v>1425</v>
+      </c>
+      <c r="G704" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H704" s="1">
+        <v>16360</v>
+      </c>
+      <c r="I704" s="2">
+        <v>559577</v>
+      </c>
+      <c r="J704" s="2">
+        <f t="shared" si="11"/>
+        <v>34.203973105134473</v>
+      </c>
+      <c r="K704" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L704" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="705" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A705">
+        <v>2015</v>
+      </c>
+      <c r="B705" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C705" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D705" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="F705" t="s">
+        <v>1427</v>
+      </c>
+      <c r="G705" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H705" s="1">
+        <v>12333</v>
+      </c>
+      <c r="I705" s="2">
+        <v>983336</v>
+      </c>
+      <c r="J705" s="2">
+        <f t="shared" si="11"/>
+        <v>79.732100867591015</v>
+      </c>
+      <c r="K705" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L705" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="706" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A706">
+        <v>2015</v>
+      </c>
+      <c r="B706" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C706" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D706" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="F706" t="s">
+        <v>1429</v>
+      </c>
+      <c r="G706" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H706" s="1">
+        <v>12696</v>
+      </c>
+      <c r="I706" s="2">
+        <v>386818</v>
+      </c>
+      <c r="J706" s="2">
+        <f t="shared" si="11"/>
+        <v>30.467706364209199</v>
+      </c>
+      <c r="K706" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L706" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="707" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A707">
+        <v>2015</v>
+      </c>
+      <c r="B707" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C707" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D707" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F707" t="s">
+        <v>1431</v>
+      </c>
+      <c r="G707" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H707" s="1">
+        <v>17343</v>
+      </c>
+      <c r="I707" s="2">
+        <v>304126</v>
+      </c>
+      <c r="J707" s="2">
+        <f t="shared" si="11"/>
+        <v>17.535951104191891</v>
+      </c>
+      <c r="K707" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L707" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="E620:F666">
     <sortCondition descending="1" ref="F620"/>

</xml_diff>